<commit_message>
Added start of graduation ceremony
</commit_message>
<xml_diff>
--- a/cambridgeBP/dialogue/npc.xlsx
+++ b/cambridgeBP/dialogue/npc.xlsx
@@ -367,9 +367,29 @@
     <t xml:space="preserve">Dean of Students</t>
   </si>
   <si>
-    <t xml:space="preserve">Welcome mathmogician I am a test!
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Welcome!
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
 We need your help with three different maths challenges.
 Pick one below, then a Professor from that school will guide you from the courtyard ahead.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Fractions</t>
@@ -746,7 +766,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -778,6 +798,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -832,7 +859,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -858,6 +885,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1046,7 +1077,7 @@
   </sheetPr>
   <dimension ref="A1:R107"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D38" activeCellId="0" sqref="D38"/>
     </sheetView>
   </sheetViews>
@@ -1861,7 +1892,7 @@
       <c r="C38" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="7" t="s">
         <v>115</v>
       </c>
       <c r="G38" s="4" t="s">

</xml_diff>

<commit_message>
Handled if player quits the game halfway through the walking bit
</commit_message>
<xml_diff>
--- a/cambridgeBP/dialogue/npc.xlsx
+++ b/cambridgeBP/dialogue/npc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="296">
   <si>
     <t xml:space="preserve">Scene</t>
   </si>
@@ -705,7 +705,7 @@
     <t xml:space="preserve">Next </t>
   </si>
   <si>
-    <t xml:space="preserve">dialogue open @e[tag=ratioNpc] @p ratioNpc6</t>
+    <t xml:space="preserve">dialogue open @e[tag=ratioNpc] @p ratioNpc2</t>
   </si>
   <si>
     <t xml:space="preserve">ratioNpc6</t>
@@ -783,9 +783,6 @@
     <t xml:space="preserve">You should know, no one has won my well game in 50 years.
  The trick to getting the coins is to mix §astronger potions §0to the §acorrect ratios.
 You'll need to make a §aNight Vision§0 potion first. Then a strong §aBreathing§0 potion to succeed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dialogue open @e[tag=ratioNpc] @p ratioNpc2</t>
   </si>
   <si>
     <t xml:space="preserve">ratioNpc9</t>
@@ -1075,32 +1072,36 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1289,1991 +1290,1991 @@
   </sheetPr>
   <dimension ref="A1:R124"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E54" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G76" activeCellId="0" sqref="G76"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F52" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J63" activeCellId="0" sqref="J63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="143.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="38.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="49.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="44.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="22.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="29.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="23.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="143.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="38.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="49.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="44.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="22.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="29.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="23.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="4" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="J11" s="4" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J15" s="3" t="s">
+      <c r="J15" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H18" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="I18" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="J18" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="I19" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J19" s="3" t="s">
+      <c r="J19" s="4" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="H22" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="I22" s="2" t="s">
+      <c r="I22" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J22" s="3" t="s">
+      <c r="J22" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H23" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="I23" s="2" t="s">
+      <c r="I23" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J23" s="3" t="s">
+      <c r="J23" s="4" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G25" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="H26" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="I26" s="2" t="s">
+      <c r="I26" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J26" s="3" t="s">
+      <c r="J26" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G27" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="H27" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="I27" s="2" t="s">
+      <c r="I27" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J27" s="3" t="s">
+      <c r="J27" s="4" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G28" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G29" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G30" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H30" s="3" t="s">
+      <c r="H30" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="I30" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J30" s="3" t="s">
+      <c r="J30" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G31" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="H31" s="3" t="s">
+      <c r="H31" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="I31" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J31" s="3" t="s">
+      <c r="J31" s="4" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="G32" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G33" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="G34" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H34" s="3" t="s">
+      <c r="H34" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="I34" s="2" t="s">
+      <c r="I34" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J34" s="2" t="s">
+      <c r="J34" s="3" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="G35" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="H35" s="3" t="s">
+      <c r="H35" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="I35" s="2" t="s">
+      <c r="I35" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J35" s="3" t="s">
+      <c r="J35" s="4" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="G36" s="3" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="G37" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D38" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="G38" s="3" t="s">
+      <c r="G38" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="H38" s="3" t="s">
+      <c r="H38" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="I38" s="3" t="s">
+      <c r="I38" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="J38" s="3" t="s">
+      <c r="J38" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="K38" s="3" t="s">
+      <c r="K38" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="L38" s="3" t="s">
+      <c r="L38" s="4" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D39" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="G39" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="H39" s="3" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="D40" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="G40" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="H40" s="3" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D41" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="G41" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="H41" s="2"/>
+      <c r="H41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D42" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="G42" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="H42" s="2"/>
+      <c r="H42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D43" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="G43" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2" t="s">
+      <c r="H43" s="3"/>
+      <c r="I43" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="J43" s="2" t="s">
+      <c r="J43" s="3" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D44" s="6" t="s">
+      <c r="D44" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="G44" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="H44" s="2" t="s">
+      <c r="H44" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="I44" s="2" t="s">
+      <c r="I44" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="J44" s="2"/>
+      <c r="J44" s="3"/>
     </row>
     <row r="45" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B45" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="C45" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="G45" s="3" t="s">
+      <c r="G45" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H45" s="3" t="s">
+      <c r="H45" s="4" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="B46" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="C46" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D46" s="0" t="s">
+      <c r="D46" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="G46" s="0" t="s">
+      <c r="G46" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="I46" s="0" t="s">
+      <c r="I46" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="J46" s="0" t="s">
+      <c r="J46" s="1" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="B47" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C47" s="0" t="s">
+      <c r="C47" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D47" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="G47" s="3" t="s">
+      <c r="G47" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="H47" s="3" t="s">
+      <c r="H47" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="I47" s="2" t="s">
+      <c r="I47" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="J47" s="2" t="s">
+      <c r="J47" s="3" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="B48" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C48" s="0" t="s">
+      <c r="C48" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D48" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="G48" s="2" t="s">
+      <c r="G48" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="H48" s="3" t="s">
+      <c r="H48" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="I48" s="2" t="s">
+      <c r="I48" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="J48" s="2" t="s">
+      <c r="J48" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="K48" s="2" t="s">
+      <c r="K48" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="L48" s="2" t="s">
+      <c r="L48" s="3" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="A49" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="B49" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C49" s="0" t="s">
+      <c r="C49" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D49" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="G49" s="3" t="s">
+      <c r="G49" s="4" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A50" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="B50" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C50" s="0" t="s">
+      <c r="C50" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D50" s="0" t="s">
+      <c r="D50" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="G50" s="2" t="s">
+      <c r="G50" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="H50" s="3" t="s">
+      <c r="H50" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="I50" s="2" t="s">
+      <c r="I50" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="J50" s="3" t="s">
+      <c r="J50" s="4" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="A51" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B51" s="0" t="s">
+      <c r="B51" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C51" s="0" t="s">
+      <c r="C51" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D51" s="0" t="s">
+      <c r="D51" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="G51" s="0" t="s">
+      <c r="G51" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="A52" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="B52" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C52" s="0" t="s">
+      <c r="C52" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D52" s="0" t="s">
+      <c r="D52" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="G52" s="2" t="s">
+      <c r="G52" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="A53" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="B53" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C53" s="0" t="s">
+      <c r="C53" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D53" s="0" t="s">
+      <c r="D53" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="G53" s="2" t="s">
+      <c r="G53" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="H53" s="3" t="s">
+      <c r="H53" s="4" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="A54" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B54" s="0" t="s">
+      <c r="B54" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C54" s="0" t="s">
+      <c r="C54" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="D54" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="G54" s="2" t="s">
+      <c r="G54" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="H54" s="3" t="s">
+      <c r="H54" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="I54" s="2" t="s">
+      <c r="I54" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J54" s="2" t="s">
+      <c r="J54" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+      <c r="A55" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B55" s="0" t="s">
+      <c r="B55" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C55" s="0" t="s">
+      <c r="C55" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D55" s="0" t="s">
+      <c r="D55" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="G55" s="0" t="s">
+      <c r="G55" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="H55" s="2" t="s">
+      <c r="H55" s="3" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+      <c r="A56" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B56" s="0" t="s">
+      <c r="B56" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C56" s="0" t="s">
+      <c r="C56" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D56" s="0" t="s">
+      <c r="D56" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="G56" s="0" t="s">
+      <c r="G56" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+      <c r="A57" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B57" s="0" t="s">
+      <c r="B57" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="0" t="s">
+      <c r="C57" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D57" s="5" t="s">
+      <c r="D57" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="G57" s="3" t="s">
+      <c r="G57" s="4" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="2" t="s">
+      <c r="A58" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C58" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="D58" s="4" t="s">
+      <c r="D58" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="G58" s="2" t="s">
+      <c r="G58" s="3" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="2" t="s">
+      <c r="A59" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C59" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="D59" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="G59" s="2" t="s">
+      <c r="G59" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="H59" s="2" t="s">
+      <c r="H59" s="3" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="2" t="s">
+      <c r="A60" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="D60" s="4" t="s">
+      <c r="D60" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="G60" s="2" t="s">
+      <c r="G60" s="3" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="2" t="s">
+      <c r="A61" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B61" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C61" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="D61" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="G61" s="2" t="s">
+      <c r="G61" s="3" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+      <c r="A62" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B62" s="0" t="s">
+      <c r="B62" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C62" s="0" t="s">
+      <c r="C62" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="D62" s="4" t="s">
+      <c r="D62" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="G62" s="2" t="s">
+      <c r="G62" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="H62" s="3" t="s">
+      <c r="H62" s="4" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+      <c r="A63" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B63" s="0" t="s">
+      <c r="B63" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C63" s="0" t="s">
+      <c r="C63" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="D63" s="0" t="s">
+      <c r="D63" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="G63" s="2" t="s">
+      <c r="G63" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="I63" s="3" t="s">
+      <c r="I63" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="J63" s="3" t="s">
+      <c r="J63" s="4" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+      <c r="A64" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B64" s="0" t="s">
+      <c r="B64" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C64" s="0" t="s">
+      <c r="C64" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="D64" s="4" t="s">
+      <c r="D64" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="G64" s="2" t="s">
+      <c r="G64" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="H64" s="3" t="s">
+      <c r="H64" s="4" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+      <c r="A65" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B65" s="0" t="s">
+      <c r="B65" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C65" s="0" t="s">
+      <c r="C65" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="D65" s="4" t="s">
+      <c r="D65" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="G65" s="2" t="s">
+      <c r="G65" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="H65" s="3" t="s">
+      <c r="H65" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="I65" s="2" t="s">
+      <c r="I65" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="J65" s="3" t="s">
+      <c r="J65" s="4" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+      <c r="A66" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B66" s="0" t="s">
+      <c r="B66" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C66" s="0" t="s">
+      <c r="C66" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="D66" s="4" t="s">
+      <c r="D66" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="G66" s="2" t="s">
+      <c r="G66" s="3" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+      <c r="A67" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B67" s="0" t="s">
+      <c r="B67" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C67" s="0" t="s">
+      <c r="C67" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="D67" s="4" t="s">
+      <c r="D67" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="G67" s="2" t="s">
+      <c r="G67" s="3" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
+      <c r="A68" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="B68" s="0" t="s">
+      <c r="B68" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C68" s="0" t="s">
+      <c r="C68" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="D68" s="4" t="s">
+      <c r="D68" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="G68" s="2" t="s">
+      <c r="G68" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="H68" s="3" t="s">
+      <c r="H68" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="I68" s="2" t="s">
+      <c r="I68" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="J68" s="2" t="s">
+      <c r="J68" s="3" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+      <c r="A69" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B69" s="0" t="s">
+      <c r="B69" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C69" s="0" t="s">
+      <c r="C69" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="D69" s="4" t="s">
+      <c r="D69" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="G69" s="2" t="s">
+      <c r="G69" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="H69" s="3" t="s">
+      <c r="H69" s="4" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="2" t="s">
+      <c r="A70" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B70" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C70" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="D70" s="4" t="s">
+      <c r="D70" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="G70" s="2" t="s">
+      <c r="G70" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="H70" s="2" t="s">
+      <c r="H70" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="3" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="71" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="2" t="s">
+      <c r="B71" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="D71" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="G71" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="H71" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="I71" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="J71" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="K71" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L71" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B72" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="C72" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="D71" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="G71" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="H71" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="I71" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="J71" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="K71" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="L71" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="2" t="s">
+      <c r="D72" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="G72" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H72" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="I72" s="3"/>
+      <c r="K72" s="3"/>
+      <c r="L72" s="3"/>
+    </row>
+    <row r="73" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B73" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C73" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="D72" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="G72" s="2" t="s">
+      <c r="D73" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
+      <c r="K73" s="3"/>
+      <c r="L73" s="3"/>
+    </row>
+    <row r="74" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="H74" s="4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="I75" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="J75" s="4" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="G76" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="H76" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="I76" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="J76" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="H77" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="I77" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="J77" s="4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="H78" s="3"/>
+    </row>
+    <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I79" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="J79" s="4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="G80" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="I80" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="J80" s="4" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A81" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H81" s="3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A82" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="G82" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="H72" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="I72" s="2"/>
-      <c r="K72" s="2"/>
-      <c r="L72" s="2"/>
-    </row>
-    <row r="73" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="D73" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="G73" s="2" t="s">
+      <c r="H82" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A83" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="G83" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="H73" s="2"/>
-      <c r="I73" s="2"/>
-      <c r="K73" s="2"/>
-      <c r="L73" s="2"/>
-    </row>
-    <row r="74" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="D74" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="G74" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="H74" s="3" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
-        <v>249</v>
-      </c>
-      <c r="B75" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="C75" s="0" t="s">
-        <v>245</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="G75" s="2" t="s">
+      <c r="H83" s="3"/>
+    </row>
+    <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G84" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="I75" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="J75" s="3" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
-        <v>252</v>
-      </c>
-      <c r="B76" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="C76" s="0" t="s">
-        <v>245</v>
-      </c>
-      <c r="D76" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="G76" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="H76" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="I76" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="J76" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
-        <v>257</v>
-      </c>
-      <c r="B77" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="C77" s="0" t="s">
-        <v>245</v>
-      </c>
-      <c r="D77" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="G77" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="H77" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="I77" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="J77" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
-        <v>262</v>
-      </c>
-      <c r="B78" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="C78" s="0" t="s">
-        <v>245</v>
-      </c>
-      <c r="D78" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="G78" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="H78" s="2"/>
-    </row>
-    <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="B79" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="C79" s="0" t="s">
-        <v>245</v>
-      </c>
-      <c r="D79" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="G79" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I79" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="J79" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
-        <v>267</v>
-      </c>
-      <c r="B80" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="C80" s="0" t="s">
-        <v>268</v>
-      </c>
-      <c r="D80" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="G80" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="I80" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="J80" s="3" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="D81" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="G81" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H81" s="2" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="D82" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="G82" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H82" s="2" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="D83" s="4" t="s">
+      <c r="H84" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B85" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="G83" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="H83" s="2"/>
-    </row>
-    <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
+      <c r="C85" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="B84" s="0" t="s">
-        <v>279</v>
-      </c>
-      <c r="C84" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="D84" s="0" t="s">
+      <c r="D85" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H85" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="G84" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="H84" s="0" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
-        <v>283</v>
-      </c>
-      <c r="B85" s="0" t="s">
-        <v>279</v>
-      </c>
-      <c r="C85" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="D85" s="0" t="s">
+    </row>
+    <row r="86" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A86" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="G85" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="H85" s="0" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="2" t="s">
+      <c r="B86" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="C86" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="B86" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="C86" s="2" t="s">
+      <c r="D86" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="D86" s="4" t="s">
+      <c r="G86" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A87" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="G86" s="2" t="s">
+      <c r="B87" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="G87" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="D87" s="4" t="s">
+    <row r="88" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A88" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="G87" s="2" t="s">
+      <c r="B88" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="G88" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="D88" s="4" t="s">
+    <row r="89" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A89" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="G88" s="2" t="s">
+      <c r="B89" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="G89" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A89" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="D89" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="G89" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D90" s="5"/>
+      <c r="D90" s="6"/>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D91" s="5"/>
+      <c r="D91" s="6"/>
     </row>
     <row r="92" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D92" s="5"/>
+      <c r="D92" s="6"/>
     </row>
     <row r="93" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D93" s="5"/>
+      <c r="D93" s="6"/>
     </row>
     <row r="94" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D94" s="5"/>
+      <c r="D94" s="6"/>
     </row>
     <row r="95" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D95" s="5"/>
+      <c r="D95" s="6"/>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D96" s="5"/>
+      <c r="D96" s="6"/>
     </row>
     <row r="97" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D97" s="5"/>
+      <c r="D97" s="6"/>
     </row>
     <row r="98" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D98" s="5"/>
+      <c r="D98" s="6"/>
     </row>
     <row r="99" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D99" s="5"/>
+      <c r="D99" s="6"/>
     </row>
     <row r="100" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D100" s="5"/>
+      <c r="D100" s="6"/>
     </row>
     <row r="101" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D101" s="5"/>
+      <c r="D101" s="6"/>
     </row>
     <row r="102" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D102" s="5"/>
+      <c r="D102" s="6"/>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D103" s="5"/>
+      <c r="D103" s="6"/>
     </row>
     <row r="104" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D104" s="5"/>
+      <c r="D104" s="6"/>
     </row>
     <row r="105" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D105" s="5"/>
+      <c r="D105" s="6"/>
     </row>
     <row r="106" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D106" s="5"/>
+      <c r="D106" s="6"/>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D107" s="5"/>
+      <c r="D107" s="6"/>
     </row>
     <row r="108" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="109" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="110" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D110" s="5"/>
+      <c r="D110" s="6"/>
     </row>
     <row r="111" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="112" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Added animation to the cauldron and renamed the game
</commit_message>
<xml_diff>
--- a/cambridgeBP/dialogue/npc.xlsx
+++ b/cambridgeBP/dialogue/npc.xlsx
@@ -401,19 +401,19 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Fractions</t>
+    <t xml:space="preserve">Keep off the grass</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent spawn:npc fraction</t>
   </si>
   <si>
-    <t xml:space="preserve">Ratios</t>
+    <t xml:space="preserve">Potion Commotion</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent spawn:npc ratio</t>
   </si>
   <si>
-    <t xml:space="preserve">Scale Factors</t>
+    <t xml:space="preserve">Window Wiz</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent spawn:npc scale</t>
@@ -1290,8 +1290,8 @@
   </sheetPr>
   <dimension ref="A1:R124"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F52" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J63" activeCellId="0" sqref="J63"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F13" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G38" activeCellId="0" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Bunch of minor edits
Changelog:

- Fixed issue where junior graduation would have senior text.
- Fixed issue with the flags not changing colour on graduation.
- Hid underside of number blocks on stands in Window game.
- Added white concrete behind empty windows.
- Fixed dialogue spacing issue in the npc in the junior dining hall.
</commit_message>
<xml_diff>
--- a/cambridgeBP/dialogue/npc.xlsx
+++ b/cambridgeBP/dialogue/npc.xlsx
@@ -401,7 +401,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Keep off the grass</t>
+    <t xml:space="preserve">Off the grass</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent spawn:npc fraction</t>
@@ -413,7 +413,7 @@
     <t xml:space="preserve">scriptevent spawn:npc ratio</t>
   </si>
   <si>
-    <t xml:space="preserve">Window Wiz</t>
+    <t xml:space="preserve">Window Whizz</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent spawn:npc scale</t>
@@ -446,7 +446,9 @@
     <t xml:space="preserve">spawnNpc5</t>
   </si>
   <si>
-    <t xml:space="preserve">I have given you and camera and portfolio, head back to each of the task areas and take pictures of what you have accomplished! The pictures will then appear in your portfolio. When you have gotten all your pictures come back and speak to me.</t>
+    <t xml:space="preserve">I have given you and camera and portfolio, head back to each of the task areas and take pictures of what you have accomplished! 
+The pictures will then appear in your portfolio. 
+When you have gotten all your pictures come back and speak to me.</t>
   </si>
   <si>
     <t xml:space="preserve">Thanks!</t>
@@ -491,7 +493,8 @@
     <t xml:space="preserve">Guild Master</t>
   </si>
   <si>
-    <t xml:space="preserve">This old building desperately needs some new windows. The architecture team needs the help of a Mathmogician to scale it correctly. Follow me!</t>
+    <t xml:space="preserve">This old building desperately needs some new windows. 
+The architecture team needs the help of a Mathmogician to scale it correctly. Follow me!</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent scale:npc 0</t>
@@ -614,10 +617,9 @@
     <t xml:space="preserve">scaleNpc9</t>
   </si>
   <si>
-    <t xml:space="preserve">Fantastic, the builders are very happy with these windows. They’ve opened up more 
-advanced windows for you to do. Now, the scale factors for these windows are a bit tricky – 
-the denominators got stuck and we can’t set them to 1, so you have to take that into account 
-when you set the numerator. Or if you want you can graduate now.</t>
+    <t xml:space="preserve">Fantastic, the builders are very happy with these windows. They’ve opened up more advanced windows for you to do. 
+The denominators got stuck and we can’t set them to 1, so you have to take that into account when you set the numerator. 
+Or if you want you can graduate now.</t>
   </si>
   <si>
     <t xml:space="preserve">scaleNpc10</t>
@@ -645,10 +647,9 @@
     <t xml:space="preserve">scaleNpc13</t>
   </si>
   <si>
-    <t xml:space="preserve">Scaling is changing size. For these windows we 
-want to scale up your design to fill the big space. We don’t want to change the shape, 
-so we scale length and width the same. Since we’re making things bigger, we’ll call 
-the original size 1 and multiply it by a whole number to make it that many times bigger. 
+    <t xml:space="preserve">Scaling is changing size. For these windows we want to scale up your design to fill the big space. 
+We don’t want to change the shape, so we scale length and width the same. 
+Since we’re making things bigger, we’ll call the original size 1 and multiply it by a whole number to make it that many times bigger. 
 The number we use is called a scale factor.</t>
   </si>
   <si>
@@ -1290,8 +1291,8 @@
   </sheetPr>
   <dimension ref="A1:R124"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F13" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G38" activeCellId="0" sqref="G38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2476,7 +2477,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="52.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
         <v>187</v>
       </c>
@@ -2556,7 +2557,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="52.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
         <v>196</v>
       </c>

</xml_diff>

<commit_message>
Added final changes to cambridge maths challenge
</commit_message>
<xml_diff>
--- a/cambridgeBP/dialogue/npc.xlsx
+++ b/cambridgeBP/dialogue/npc.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28029"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C2D45BA-2388-479B-83D6-F62807F0A93E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB9A3761-E300-4C7A-9740-4299FC1CE594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="298">
   <si>
     <t>Scene</t>
   </si>
@@ -138,6 +138,12 @@
     <t>Thanks for rescuing me!</t>
   </si>
   <si>
+    <t>Graduate</t>
+  </si>
+  <si>
+    <t>scriptevent graduation:junior</t>
+  </si>
+  <si>
     <t>rodNpc1Win</t>
   </si>
   <si>
@@ -238,12 +244,6 @@
   </si>
   <si>
     <t>scriptevent rod:npcComplete 4</t>
-  </si>
-  <si>
-    <t>Graduate</t>
-  </si>
-  <si>
-    <t>scriptevent graduation:junior</t>
   </si>
   <si>
     <t>rodNpc4Fail</t>
@@ -500,7 +500,7 @@
     <t>scaleNpc</t>
   </si>
   <si>
-    <t>Guild Master</t>
+    <t>Guild Leader</t>
   </si>
   <si>
     <t>This old building desperately needs some new windows. 
@@ -666,8 +666,8 @@
     <t>scaleNpc14</t>
   </si>
   <si>
-    <t>You'll need to change the §anumerator§0 (the top number) to scale the windows.
-To make the window larger you'll need to make the §anumerator larger§0 than the denominator (bottom number).
+    <t>You'll need to change the §1numerator§0 (the top number) to scale the windows.
+To make the window larger you'll need to make the §1numerator larger§0 than the denominator (bottom number).
  The windows must fit in the frame! So make sure you don't make the windows too big.</t>
   </si>
   <si>
@@ -743,6 +743,12 @@
   </si>
   <si>
     <t>dialogue open @e[tag=ratioNpc] @p ratioNpc4</t>
+  </si>
+  <si>
+    <t>Repeat Chat</t>
+  </si>
+  <si>
+    <t>dialogue open @e[tag=ratioNpc] @p ratioNpc8</t>
   </si>
   <si>
     <t>ratioNpc4</t>
@@ -774,9 +780,6 @@
     <t>scriptevent ratio:npc 3</t>
   </si>
   <si>
-    <t>dialogue open @e[tag=ratioNpc] @p ratioNpc8</t>
-  </si>
-  <si>
     <t>ratioNpc7</t>
   </si>
   <si>
@@ -792,8 +795,8 @@
   </si>
   <si>
     <t>You should know, no one has won my well game in 50 years.
- The trick to getting the coins is to mix §astronger potions §0to the §acorrect ratios.
-You'll need to make a §aNight Vision§0 potion first. Then a strong §aBreathing§0 potion to succeed.</t>
+ The trick to getting the coins is to mix §1stronger potions §0to the §1correct ratios.
+You'll need to make a §1Night Vision§0 potion first. Then a strong §1Breathing§0 potion to succeed.</t>
   </si>
   <si>
     <t>ratioNpc9</t>
@@ -919,8 +922,8 @@
     <t>fractionNpc8</t>
   </si>
   <si>
-    <t>You §acan't jump or step on the grass §0in the gardens. 
-You'll be told off if you do! I'll give you §adifferent sized magical rods§0 to cross the gaps to save the students. Two gardens are §a24x24§0 blocks wide and one is §a24x48§0. Each gap will be a fraction of 24.</t>
+    <t>You §1can't jump or step on the grass §0in the gardens. 
+You'll be told off if you do! I'll give you §1different sized magical rods§0 to cross the gaps to save the students. Two gardens are §124x24§0 blocks wide and one is §124x48§0. Each gap will be a fraction of 24.</t>
   </si>
   <si>
     <t>dialogue open @e[tag=fractionNpc] @p fractionNpc2</t>
@@ -1268,8 +1271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E52" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I75" sqref="I75"/>
+    <sheetView tabSelected="1" topLeftCell="D54" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L65" sqref="L65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75"/>
@@ -1429,36 +1432,42 @@
       <c r="G5" t="s">
         <v>22</v>
       </c>
+      <c r="I5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>25</v>
@@ -1467,24 +1476,24 @@
         <v>26</v>
       </c>
       <c r="H7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>28</v>
       </c>
       <c r="J7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>30</v>
@@ -1495,13 +1504,13 @@
     </row>
     <row r="9" spans="1:18">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>33</v>
@@ -1509,36 +1518,42 @@
       <c r="G9" t="s">
         <v>22</v>
       </c>
+      <c r="I9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="10" spans="1:18" ht="18" customHeight="1">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>25</v>
@@ -1547,24 +1562,24 @@
         <v>26</v>
       </c>
       <c r="H11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>28</v>
       </c>
       <c r="J11" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
         <v>30</v>
@@ -1575,13 +1590,13 @@
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D13" t="s">
         <v>33</v>
@@ -1589,36 +1604,42 @@
       <c r="G13" t="s">
         <v>22</v>
       </c>
+      <c r="I13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="14" spans="1:18" ht="15" customHeight="1">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="17.25" customHeight="1">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>25</v>
@@ -1627,24 +1648,24 @@
         <v>26</v>
       </c>
       <c r="H15" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>28</v>
       </c>
       <c r="J15" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="17.25" customHeight="1">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>30</v>
@@ -1655,13 +1676,13 @@
     </row>
     <row r="17" spans="1:10" ht="17.25" customHeight="1">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D17" t="s">
         <v>33</v>
@@ -1669,31 +1690,37 @@
       <c r="G17" t="s">
         <v>22</v>
       </c>
+      <c r="I17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="18" spans="1:10" ht="17.25" customHeight="1">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="17.25" customHeight="1">
@@ -1701,10 +1728,10 @@
         <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>25</v>
@@ -1719,7 +1746,7 @@
         <v>28</v>
       </c>
       <c r="J19" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="17.25" customHeight="1">
@@ -1727,10 +1754,10 @@
         <v>73</v>
       </c>
       <c r="B20" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>30</v>
@@ -1744,16 +1771,22 @@
         <v>74</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D21" t="s">
         <v>33</v>
       </c>
       <c r="G21" t="s">
         <v>22</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="17.25" customHeight="1">
@@ -1770,16 +1803,16 @@
         <v>78</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H22" t="s">
         <v>79</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="J22" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="18" customHeight="1">
@@ -1841,6 +1874,12 @@
       <c r="G25" t="s">
         <v>22</v>
       </c>
+      <c r="I25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="26" spans="1:10" ht="18" customHeight="1">
       <c r="A26" t="s">
@@ -1862,10 +1901,10 @@
         <v>89</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="J26" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1908,7 +1947,7 @@
         <v>33</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="16.5" customHeight="1">
@@ -1942,16 +1981,16 @@
         <v>97</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H30" t="s">
         <v>98</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="J30" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="16.5" customHeight="1">
@@ -1994,7 +2033,13 @@
         <v>33</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="16.5" customHeight="1">
@@ -2028,7 +2073,7 @@
         <v>106</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="H34" t="s">
         <v>107</v>
@@ -2470,10 +2515,10 @@
         <v>176</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="18" customHeight="1">
@@ -2490,7 +2535,7 @@
         <v>190</v>
       </c>
       <c r="G55" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>107</v>
@@ -2547,7 +2592,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="37.35">
+    <row r="59" spans="1:10" ht="48.75">
       <c r="A59" s="2" t="s">
         <v>198</v>
       </c>
@@ -2689,10 +2734,16 @@
       <c r="J65" t="s">
         <v>222</v>
       </c>
+      <c r="K65" t="s">
+        <v>223</v>
+      </c>
+      <c r="L65" s="2" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="66" spans="1:12" ht="18" customHeight="1">
       <c r="A66" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B66" t="s">
         <v>205</v>
@@ -2701,7 +2752,7 @@
         <v>206</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>172</v>
@@ -2709,7 +2760,7 @@
     </row>
     <row r="67" spans="1:12" ht="18" customHeight="1">
       <c r="A67" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B67" t="s">
         <v>205</v>
@@ -2718,7 +2769,7 @@
         <v>206</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>153</v>
@@ -2726,7 +2777,7 @@
     </row>
     <row r="68" spans="1:12" ht="18" customHeight="1">
       <c r="A68" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B68" t="s">
         <v>205</v>
@@ -2735,24 +2786,24 @@
         <v>206</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="G68" s="2" t="s">
         <v>195</v>
       </c>
       <c r="H68" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="I68" s="2" t="s">
         <v>160</v>
       </c>
       <c r="J68" s="2" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="69" spans="1:12" ht="18" customHeight="1">
       <c r="A69" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B69" t="s">
         <v>205</v>
@@ -2761,18 +2812,18 @@
         <v>206</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>195</v>
       </c>
       <c r="H69" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="70" spans="1:12" ht="18" customHeight="1">
       <c r="A70" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>205</v>
@@ -2781,7 +2832,7 @@
         <v>206</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>88</v>
@@ -2792,7 +2843,7 @@
     </row>
     <row r="71" spans="1:12" ht="18" customHeight="1">
       <c r="A71" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B71" t="s">
         <v>205</v>
@@ -2801,7 +2852,7 @@
         <v>206</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>220</v>
@@ -2816,15 +2867,15 @@
         <v>222</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="L71" s="2" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
     </row>
     <row r="72" spans="1:12" ht="18" customHeight="1">
       <c r="A72" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>205</v>
@@ -2833,7 +2884,7 @@
         <v>206</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>88</v>
@@ -2847,7 +2898,7 @@
     </row>
     <row r="73" spans="1:12" ht="18" customHeight="1">
       <c r="A73" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>205</v>
@@ -2856,7 +2907,7 @@
         <v>206</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>135</v>
@@ -2868,36 +2919,36 @@
     </row>
     <row r="74" spans="1:12" ht="18" customHeight="1">
       <c r="A74" s="4" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B74" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C74" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="H74" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="75" spans="1:12" ht="18" customHeight="1">
       <c r="A75" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B75" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C75" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>153</v>
@@ -2906,73 +2957,73 @@
         <v>154</v>
       </c>
       <c r="J75" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="76" spans="1:12" ht="18" customHeight="1">
       <c r="A76" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B76" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C76" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="G76" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H76" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="I76" s="2" t="s">
         <v>160</v>
       </c>
       <c r="J76" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="77" spans="1:12" ht="15.75" customHeight="1">
       <c r="A77" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B77" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C77" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>163</v>
       </c>
       <c r="G77" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H77" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="I77" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="J77" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="78" spans="1:12" ht="15.75" customHeight="1">
       <c r="A78" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B78" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C78" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="G78" t="s">
         <v>172</v>
@@ -2981,102 +3032,108 @@
     </row>
     <row r="79" spans="1:12" ht="15.75" customHeight="1">
       <c r="A79" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B79" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C79" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G79" t="s">
         <v>31</v>
       </c>
       <c r="I79" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="J79" t="s">
-        <v>260</v>
+        <v>261</v>
+      </c>
+      <c r="K79" t="s">
+        <v>223</v>
+      </c>
+      <c r="L79" s="2" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="80" spans="1:12" ht="15.75" customHeight="1">
       <c r="A80" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B80" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C80" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G80" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="I80" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="J80" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="15.75" customHeight="1">
       <c r="A81" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G81" s="2" t="s">
         <v>31</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="15.75" customHeight="1">
       <c r="A82" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>88</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="15.75" customHeight="1">
       <c r="A83" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>135</v>
@@ -3085,56 +3142,56 @@
     </row>
     <row r="84" spans="1:8" ht="15.75" customHeight="1">
       <c r="A84" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B84" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C84" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D84" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="G84" t="s">
         <v>153</v>
       </c>
       <c r="H84" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="16.5" customHeight="1">
       <c r="A85" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B85" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C85" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D85" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="G85" t="s">
         <v>153</v>
       </c>
       <c r="H85" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="16.5" customHeight="1">
       <c r="A86" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="G86" s="2" t="s">
         <v>132</v>
@@ -3142,16 +3199,16 @@
     </row>
     <row r="87" spans="1:8" ht="17.25" customHeight="1">
       <c r="A87" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="G87" s="2" t="s">
         <v>132</v>
@@ -3159,16 +3216,16 @@
     </row>
     <row r="88" spans="1:8" ht="17.25" customHeight="1">
       <c r="A88" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="G88" s="2" t="s">
         <v>132</v>
@@ -3176,16 +3233,16 @@
     </row>
     <row r="89" spans="1:8" ht="17.25" customHeight="1">
       <c r="A89" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="G89" s="2" t="s">
         <v>132</v>

</xml_diff>

<commit_message>
Added text from cambridge
</commit_message>
<xml_diff>
--- a/cambridgeBP/dialogue/npc.xlsx
+++ b/cambridgeBP/dialogue/npc.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28103"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB9A3761-E300-4C7A-9740-4299FC1CE594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{081C2F3C-EA30-4529-86E1-F49349F2275B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="310">
   <si>
     <t>Scene</t>
   </si>
@@ -99,7 +99,7 @@
     <t>Annie</t>
   </si>
   <si>
-    <t>Great work, the garden is 24 across and I am halfway along. So using the 12 rod is exactly right. Thank you for saving me.</t>
+    <t>Great work, the garden is 1 td (24 blocks) across and I am halfway along. So the 1/2 td rod (12 blocks) fits perfectly! Thank you for saving me.</t>
   </si>
   <si>
     <t>No problem!</t>
@@ -120,13 +120,19 @@
     <t>scriptevent rod:npcReplay 0</t>
   </si>
   <si>
+    <t>I’ll work it out</t>
+  </si>
+  <si>
+    <t>scriptevent rod:noReplay 0</t>
+  </si>
+  <si>
     <t>I’ll carry on</t>
   </si>
   <si>
     <t>rodNpc0Default</t>
   </si>
   <si>
-    <t>Help me! You can only rescue me if you use the right amount of rods to get to this platform, otherwise I can't get back safely. If you need to start again talk to the Prof.</t>
+    <t>Help me! You can only rescue me if you reach this platform, otherwise I can't get back safely. If you need to start again talk to the Prof.</t>
   </si>
   <si>
     <t>Okay</t>
@@ -153,7 +159,7 @@
     <t>Lisa</t>
   </si>
   <si>
-    <t>You saved me! 12 is half of 24 and you used the right rod to get here.</t>
+    <t>You saved me! 12 blocks is half of 1 td (24 blocks) and you used the fewest rods to get here.</t>
   </si>
   <si>
     <t>You’re Welcome</t>
@@ -168,6 +174,9 @@
     <t>scriptevent rod:npcReplay 1</t>
   </si>
   <si>
+    <t>scriptevent rod:noReplay 1</t>
+  </si>
+  <si>
     <t>rodNpc1Default</t>
   </si>
   <si>
@@ -183,7 +192,7 @@
     <t>Callum</t>
   </si>
   <si>
-    <t>You saved me! 4 is a sixth of 24 and you used the right rod to get here.</t>
+    <t>You saved me! the 4-block rod is 1/6 of 1 td and you used the fewest rods to get here.</t>
   </si>
   <si>
     <t>scriptevent rod:npcComplete 2</t>
@@ -192,9 +201,18 @@
     <t>rodNpc2Fail</t>
   </si>
   <si>
+    <t>You saved me! However, that's not the solution that uses the fewest rods. Do you want me to show you?</t>
+  </si>
+  <si>
     <t>scriptevent rod:npcReplay 2</t>
   </si>
   <si>
+    <t>I’ll work it out.</t>
+  </si>
+  <si>
+    <t>scriptevent rod:noReplay 2</t>
+  </si>
+  <si>
     <t>rodNpc2Default</t>
   </si>
   <si>
@@ -210,7 +228,7 @@
     <t>Deena</t>
   </si>
   <si>
-    <t>Great work you made ¾ in the most optimum way by combining  ½ and ¼ .</t>
+    <t>Great work you made ¾ by using ½ and ¼ , and you used the fewest rods to get here.</t>
   </si>
   <si>
     <t>scriptevent rod:npcComplete 3</t>
@@ -222,6 +240,9 @@
     <t>scriptevent rod:npcReplay 3</t>
   </si>
   <si>
+    <t>scriptevent rod:noReplay 3</t>
+  </si>
+  <si>
     <t>rodNpc3Default</t>
   </si>
   <si>
@@ -237,7 +258,7 @@
     <t>Eli</t>
   </si>
   <si>
-    <t>Well done! You combined ¼ with 1/8 to make 3/8.</t>
+    <t>Well done! You used ¼ with 1/8 to make 3/8, and you used smallest number of rods to get here.</t>
   </si>
   <si>
     <t>Great</t>
@@ -255,6 +276,9 @@
     <t>scriptevent rod:npcReplay 4</t>
   </si>
   <si>
+    <t>scriptevent rod:noReplay 4</t>
+  </si>
+  <si>
     <t>rodNpc4Default</t>
   </si>
   <si>
@@ -270,7 +294,7 @@
     <t>Isaac</t>
   </si>
   <si>
-    <t>Wow, great working going over 1 tweed.</t>
+    <t>Wow, great work, you covered a distance greater than 1 td and you used smallest number of rods to get here.</t>
   </si>
   <si>
     <t>scriptevent rod:npcComplete 5</t>
@@ -282,6 +306,9 @@
     <t>scriptevent rod:npcReplay 5</t>
   </si>
   <si>
+    <t>scriptevent rod:noReplay 5</t>
+  </si>
+  <si>
     <t>rodNpc5Default</t>
   </si>
   <si>
@@ -297,7 +324,7 @@
     <t>Tamsin</t>
   </si>
   <si>
-    <t>Well done, 3/1 is 36, great work.</t>
+    <t>Well done! You went 3/2 td (36 blocks) by using the 1 td and 1/2 td rods, and you used the fewest rods to get here.</t>
   </si>
   <si>
     <t>Thanks</t>
@@ -312,6 +339,9 @@
     <t>scriptevent rod:npcReplay 6</t>
   </si>
   <si>
+    <t>scriptevent rod:noReplay 6</t>
+  </si>
+  <si>
     <t>rodNpc6Saved</t>
   </si>
   <si>
@@ -327,7 +357,7 @@
     <t>Fleur</t>
   </si>
   <si>
-    <t>You saved me! 3 is indeed 1/8 of 24, you used the right rod.</t>
+    <t>You saved me! 1/8 of 1 td is indeed 3 blocks, and you used the fewest rods to get here.</t>
   </si>
   <si>
     <t>scriptevent rod:npcComplete 7</t>
@@ -339,6 +369,9 @@
     <t>scriptevent rod:npcReplay 7</t>
   </si>
   <si>
+    <t>scriptevent rod:noReplay 7</t>
+  </si>
+  <si>
     <t>rodNpc7Saved</t>
   </si>
   <si>
@@ -367,6 +400,9 @@
   </si>
   <si>
     <t>scriptevent rod:npcReplay 8</t>
+  </si>
+  <si>
+    <t>scriptevent rod:noReplay 8</t>
   </si>
   <si>
     <t>scriptevent rod:npcComplete 8</t>
@@ -406,7 +442,7 @@
         <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">
-We need your help with three different maths challenges.
+We need your help with three different mathematics challenges.
 Pick one below, then a Professor from that school will guide you from the courtyard ahead.</t>
     </r>
   </si>
@@ -432,7 +468,7 @@
     <t>spawnNpc2</t>
   </si>
   <si>
-    <t>Congratulations on graduating! You have received the junior award. You can try again to see if you can get the senior degree, or try another challenge.</t>
+    <t>Congratulations on graduating! You have received the junior degree and are now Second Proportion Wrangler. You can try again to aim for the senior degree, or try another challenge.</t>
   </si>
   <si>
     <t>scriptevent graduation:finale</t>
@@ -441,7 +477,7 @@
     <t>spawnNpc3</t>
   </si>
   <si>
-    <t>Congratulations on graduating! You have received the senior award, our highest degree! Feel free to try the other challenges.</t>
+    <t>Congratulations on graduating! You have received the senior award, our highest degree, and are now Senior Proportion Wrangler! Feel free to try the other challenges.</t>
   </si>
   <si>
     <t>spawnNpc4</t>
@@ -458,7 +494,7 @@
   <si>
     <t>I have given you and camera and portfolio, head back to each of the task areas and take pictures of what you have accomplished! 
 The pictures will then appear in your portfolio. 
-When you have gotten all your pictures come back and speak to me.</t>
+When you have taken all your pictures come back and speak to me.</t>
   </si>
   <si>
     <t>Thanks!</t>
@@ -529,8 +565,8 @@
   </si>
   <si>
     <t>The design has already been done, but I need your help to scale it. 
-Click on the numerator (top number) to change the scale size. You can count the number of blocks in the frame to work it out. 
-Then click on the orb of scaling to my right, to scale the window.</t>
+Click on the numerator (top number) to change the scale factor size. To figure it out, you can count how many of the smaller window's widths would fit into the bigger window's width. 
+Then click on the orb of scaling to my right, to §1scale up§0 the window.</t>
   </si>
   <si>
     <t>Will do</t>
@@ -573,10 +609,10 @@
   </si>
   <si>
     <t>1. Place the stained glass in the frames.
-2. Left click the numerator (top number) with the wand to change it.
-3. Count the blocks under the window to work out each scale factor.
+2. How many of the smaller window's §1widths§0 would fit into the bigger window's §1width§0? That's the §1scale factor§0.
+3. Left click the §1numerator§0 (top number) with the wand to change the §1scale factor§0.
 4. Right click the pink and blue orb to make the window appear.
-5. If you’ve made a mistake change the numerator and right click the orb.</t>
+5. If you’ve made a mistake change the §1numerator§0 and right click the orb again.</t>
   </si>
   <si>
     <t>Thank you</t>
@@ -585,7 +621,7 @@
     <t>scaleNpc5</t>
   </si>
   <si>
-    <t>That window fits beautifully! Do you want to keep it and move on or redesign it?</t>
+    <t>That window fits beautifully! Do you want to keep it and move on or redesign the glass?</t>
   </si>
   <si>
     <t>Carry on</t>
@@ -628,7 +664,7 @@
   </si>
   <si>
     <t>Fantastic, the builders are very happy with these windows. They’ve opened up more advanced windows for you to do. 
-The denominators got stuck and we can’t set them to 1, so you have to take that into account when you set the numerator. 
+The §1denominators§0 got stuck and we can't set them to 1, so remember that when setting the §1numerator§0. You still want the §1scale factor§0 to be §1equivalent§0 to a §1whole number§0!
 Or if you want you can graduate now.</t>
   </si>
   <si>
@@ -647,8 +683,8 @@
     <t>scaleNpc12</t>
   </si>
   <si>
-    <t>We’re working in blocks here, that scale factor isn’t a whole number. 
-Try again but make it a whole number.</t>
+    <t>We’re working in blocks here, that §1scale factor§0 isn’t a §1whole number§0. 
+Try again, but the §1scale factor§0 has to be §1equivalent§0 to a §1whole number§0.</t>
   </si>
   <si>
     <t>On it!</t>
@@ -657,27 +693,24 @@
     <t>scaleNpc13</t>
   </si>
   <si>
-    <t>Scaling is changing size. For these windows we want to scale up your design to fill the big space. 
-We don’t want to change the shape, so we scale length and width the same. 
-Since we’re making things bigger, we’ll call the original size 1 and multiply it by a whole number to make it that many times bigger. 
-The number we use is called a scale factor.</t>
+    <t xml:space="preserve">§1Scaling§0 is changing size. For these windows we want to §1scale up§0 your design to fill the bigger space. 
+We don’t want to change the shape, so we scale §1height§0 and §1width§0 the same. 
+Since want to make things bigger, we’ll call the original size 1 and multiply it by a §1whole number§0 §1scale factor§0, to make it that many times bigger. </t>
   </si>
   <si>
     <t>scaleNpc14</t>
   </si>
   <si>
-    <t>You'll need to change the §1numerator§0 (the top number) to scale the windows.
-To make the window larger you'll need to make the §1numerator larger§0 than the denominator (bottom number).
- The windows must fit in the frame! So make sure you don't make the windows too big.</t>
+    <t>You'll need to change the §1numerator§0 (the top number) to §1scale up§0 the windows.
+To make the window larger you'll need to make the §1numerator§0 larger than the §1denominator§0 (bottom number).
+ The windows must fit in the frame!</t>
   </si>
   <si>
     <t>scaleNpc15</t>
   </si>
   <si>
     <t>Fantastic, the builders are very happy with these windows. They’ve opened up more 
-advanced windows for you to do. Now, the scale factors for these windows are a bit tricky – 
-the denominators got stuck and we can’t set them to 1, so you have to take that into account 
-when you set the numerator.</t>
+advanced windows for you to do. Now, the §1scale factors§0 for these windows are a bit tricky –  the §1denominators§0 got stuck and we can't set them to 1, so remember that when setting the §1numerators§0. You still want each scale factor to be equivalent to a whole number!</t>
   </si>
   <si>
     <t>scaleNpc16</t>
@@ -695,7 +728,7 @@
     <t>Professor of Alchemy</t>
   </si>
   <si>
-    <t xml:space="preserve">I hear you want to take on the Well diving championship, very well, follow me. </t>
+    <t xml:space="preserve">I hear you want to take part in the well-diving championship, very well, follow me. </t>
   </si>
   <si>
     <t>Let's Go</t>
@@ -723,7 +756,7 @@
   </si>
   <si>
     <t>Mmmm delicious, okay lets get some coins.
-The ratios for the potions you’ll need are on the wall. 
+The §1ratios§0 for the potions you’ll need are on the wall. 
 To make a potion mix it in the cauldron and tap it with your wand.</t>
   </si>
   <si>
@@ -755,12 +788,13 @@
   </si>
   <si>
     <t>Here are the steps for the game. 
-1. Check the ratios on the wall.
-2. Throw the ingredients in the cauldron to the correct ratio.
+1. Check the §1ratios§0 on the wall.
+2. Throw the ingredients in the cauldron, in the correct §1ratio§0.
 3. Click on the cauldron with your wand.
-4. Check the bar chart to see if your ratios are correct. 
+4. Check the §1bar chart§0 to see if your §1ratios§0 are correct. 
 5. If they are correct, drink the potion and dive in the well. 
-6. Remember to follow the rules, and click on the coins to gather them!</t>
+6. Remember to follow the rules, and click on the coins to gather them!
+7. If you can't get all the coins, try a different type of potion, or maybe make a bigger batch!</t>
   </si>
   <si>
     <t>ratioNpc5</t>
@@ -772,7 +806,7 @@
     <t>ratioNpc2</t>
   </si>
   <si>
-    <t>Before we start I need you to make me a .... 
+    <t>Before we start I need you to make me a... 
 I mean teach you about ratios, by making me chocolate milk. 
 Put 2 parts Cocoa beans to 1 part Milk into the cauldron and tap it with your wand.</t>
   </si>
@@ -795,8 +829,8 @@
   </si>
   <si>
     <t>You should know, no one has won my well game in 50 years.
- The trick to getting the coins is to mix §1stronger potions §0to the §1correct ratios.
-You'll need to make a §1Night Vision§0 potion first. Then a strong §1Breathing§0 potion to succeed.</t>
+ The trick to getting the coins is to mix §1each potion §0in the §1correct ratio. If it isn't strong enough, make a bigger batch!
+You'll need to make a §1Night Vision§0 potion first. Then a BIG batch of §1Breathing§0 potion to succeed.</t>
   </si>
   <si>
     <t>ratioNpc9</t>
@@ -808,7 +842,7 @@
     <t>ratioNpc10</t>
   </si>
   <si>
-    <t>Well done! You got all of the coins, good job. You can head on over to the graduation!</t>
+    <t>Well done! You got all of the coins and are now the Well-Diving Champion. You can head on over to the graduation!</t>
   </si>
   <si>
     <t>ratioNpc11</t>
@@ -848,7 +882,7 @@
   </si>
   <si>
     <t>I need you to rescue each student that is trapped.  Use these magical rods to reach each student. 
-If you need to start again or get stuck come back to me!</t>
+If you get stuck or need to start again!</t>
   </si>
   <si>
     <t>Wish me luck</t>
@@ -869,7 +903,7 @@
     <t>dialogue open @e[tag=fractionNpc] @p fractionNpc4</t>
   </si>
   <si>
-    <t>Start Again</t>
+    <t>Start again</t>
   </si>
   <si>
     <t>dialogue open @e[tag=fractionNpc] @p fractionNpc6</t>
@@ -878,19 +912,21 @@
     <t>fractionNpc4</t>
   </si>
   <si>
-    <t>1. All the fractions are of 24 as two of the rooms are 24x24 blocks wide, and one is 48x24. You need to use the rods to cross them.
-2. You can place the rods by right clicking in front of the white blocks. 
-3. Talk to each student as you go, they will let you know if you have placed the most optimum rod down. 
-4. You won't be able to jump, and walking on the grass is forbidden!</t>
+    <t>1. You need to cross the grass on the fraction rods to rescue students. 
+2. All the rod lengths are fractions of 1 td (24 blocks). 
+3. We have limited rods so you need to use as few as possible!
+4. You can place the rods by right clicking in front of the white blocks. 
+5. Talk to each student as you go, they will let you know if you have used the fewest rods to rescue them. 
+6. You won't be able to jump, and walking on the grass is forbidden!</t>
   </si>
   <si>
     <t>fractionNpc5</t>
   </si>
   <si>
-    <t>Well done you saved the student and made it to a checkpoint. Come back to me if you run out of rods.</t>
-  </si>
-  <si>
-    <t>More Rods</t>
+    <t>Well done, you saved the student and made it to a checkpoint. Come back to me if you run out of rods.</t>
+  </si>
+  <si>
+    <t>More rods</t>
   </si>
   <si>
     <t>fractionNpc6</t>
@@ -899,7 +935,8 @@
     <t xml:space="preserve">Professor of Cartography </t>
   </si>
   <si>
-    <t>Getting more rods will reset the game. 
+    <t>We only have a fixed number of rods for this challenge. 
+Getting more rods will reset the game. 
 Are you sure you want to reset the game?</t>
   </si>
   <si>
@@ -916,14 +953,14 @@
   </si>
   <si>
     <t>Around here, we measure distance in Tweeds (td). 1 td = 24 blocks. 
-We have rods that are different fractions of 1 td. We don’t have too many, so use them carefully! You have just enough to rescue everyone.</t>
+We have rods with lengths that are different §1fractions§0 of 1 td. We don’t have too many, so try to use as few rods as you can to rescue each student!</t>
   </si>
   <si>
     <t>fractionNpc8</t>
   </si>
   <si>
     <t>You §1can't jump or step on the grass §0in the gardens. 
-You'll be told off if you do! I'll give you §1different sized magical rods§0 to cross the gaps to save the students. Two gardens are §124x24§0 blocks wide and one is §124x48§0. Each gap will be a fraction of 24.</t>
+You'll be told off if you do! I'll give you different-sized magical rods to cross the gaps to save the students. Two gardens are 1 td x 1 td wide and one is 1 td x 2 td wide. The §1length§0 of each rod is a §1fraction§0 of 1 td (1 td = 24 blocks).</t>
   </si>
   <si>
     <t>dialogue open @e[tag=fractionNpc] @p fractionNpc2</t>
@@ -1058,7 +1095,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1072,6 +1109,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1271,8 +1311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D54" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L65" sqref="L65"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75"/>
@@ -1288,7 +1328,7 @@
     <col min="9" max="9" width="18.875" customWidth="1"/>
     <col min="10" max="10" width="49.125" customWidth="1"/>
     <col min="11" max="11" width="20" customWidth="1"/>
-    <col min="12" max="12" width="24" customWidth="1"/>
+    <col min="12" max="12" width="31" customWidth="1"/>
     <col min="13" max="13" width="10.5" customWidth="1"/>
     <col min="14" max="14" width="44.625" customWidth="1"/>
     <col min="15" max="15" width="22.875" customWidth="1"/>
@@ -1396,12 +1436,18 @@
         <v>28</v>
       </c>
       <c r="J3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
@@ -1410,15 +1456,15 @@
         <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
@@ -1427,47 +1473,47 @@
         <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>25</v>
@@ -1476,170 +1522,182 @@
         <v>26</v>
       </c>
       <c r="H7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>28</v>
       </c>
       <c r="J7" t="s">
-        <v>41</v>
+        <v>46</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:18">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G9" t="s">
         <v>22</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="18" customHeight="1">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H10" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1">
       <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="D11" s="3" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>26</v>
       </c>
       <c r="H11" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="J11" t="s">
-        <v>50</v>
+        <v>58</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L11" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G13" t="s">
         <v>22</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="15" customHeight="1">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H14" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="17.25" customHeight="1">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>25</v>
@@ -1648,1249 +1706,1285 @@
         <v>26</v>
       </c>
       <c r="H15" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>28</v>
       </c>
       <c r="J15" t="s">
-        <v>59</v>
+        <v>68</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L15" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="17.25" customHeight="1">
       <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" t="s">
         <v>62</v>
       </c>
-      <c r="B16" t="s">
-        <v>56</v>
-      </c>
       <c r="C16" s="2" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="17.25" customHeight="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="17.25" customHeight="1">
       <c r="A17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B17" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G17" t="s">
         <v>22</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="17.25" customHeight="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="17.25" customHeight="1">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="H18" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="17.25" customHeight="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="17.25" customHeight="1">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="H19" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>28</v>
       </c>
       <c r="J19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="17.25" customHeight="1">
+        <v>80</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="17.25" customHeight="1">
       <c r="A20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B20" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="D20" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="17.25" customHeight="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="17.25" customHeight="1">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G21" t="s">
         <v>22</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="17.25" customHeight="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="17.25" customHeight="1">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="C22" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H22" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="18" customHeight="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="18" customHeight="1">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B23" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="C23" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="H23" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>28</v>
       </c>
       <c r="J23" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="18" customHeight="1">
+        <v>90</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="18" customHeight="1">
       <c r="A24" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="B24" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="C24" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="18" customHeight="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="18" customHeight="1">
       <c r="A25" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="B25" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G25" t="s">
         <v>22</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="18" customHeight="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="18" customHeight="1">
       <c r="A26" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="B26" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="C26" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="H26" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="16.5">
       <c r="A27" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B27" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="C27" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="H27" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>28</v>
       </c>
       <c r="J27" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
+        <v>101</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L27" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="B28" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="C28" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="D28" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A29" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G29" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G28" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A29" t="s">
-        <v>93</v>
-      </c>
-      <c r="B29" t="s">
-        <v>85</v>
-      </c>
-      <c r="C29" t="s">
-        <v>86</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="16.5" customHeight="1">
+    </row>
+    <row r="30" spans="1:12" ht="16.5" customHeight="1">
       <c r="A30" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="B30" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H30" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J30" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="16.5" customHeight="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="16.5" customHeight="1">
       <c r="A31" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="H31" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>28</v>
       </c>
       <c r="J31" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="16.5" customHeight="1">
+        <v>111</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L31" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="16.5" customHeight="1">
       <c r="A32" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="B32" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="16.5" customHeight="1">
       <c r="A33" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="B33" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="16.5" customHeight="1">
       <c r="A34" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="B34" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H34" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" ht="16.5">
       <c r="A35" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="B35" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="H35" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="I35" s="2" t="s">
         <v>28</v>
       </c>
       <c r="J35" t="s">
-        <v>111</v>
+        <v>122</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L35" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="36" spans="1:12">
       <c r="A36" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="B36" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="15.75" customHeight="1">
       <c r="A37" t="s">
+        <v>127</v>
+      </c>
+      <c r="B37" t="s">
         <v>115</v>
       </c>
-      <c r="B37" t="s">
-        <v>104</v>
-      </c>
       <c r="C37" s="2" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="17.25" customHeight="1">
       <c r="A38" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="B38" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="G38" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="H38" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="I38" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="J38" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="K38" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="L38" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="17.25" customHeight="1">
       <c r="A39" s="2" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="17.25" customHeight="1">
       <c r="A40" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>116</v>
-      </c>
       <c r="C40" s="2" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="17.25" customHeight="1">
       <c r="A41" s="2" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="H41" s="2"/>
     </row>
     <row r="42" spans="1:12" ht="17.25" customHeight="1">
       <c r="A42" s="2" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="H42" s="2"/>
     </row>
     <row r="43" spans="1:12" ht="17.25" customHeight="1">
       <c r="A43" s="2" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="2" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="17.25" customHeight="1">
       <c r="A44" s="2" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="J44" s="2"/>
     </row>
     <row r="45" spans="1:12" ht="17.25" customHeight="1">
       <c r="A45" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
       <c r="B45" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="C45" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="G45" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H45" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="17.25" customHeight="1">
       <c r="A46" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="B46" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="C46" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="D46" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="G46" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="I46" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="J46" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="17.25" customHeight="1">
       <c r="A47" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="B47" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="C47" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="G47" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="H47" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
     </row>
     <row r="48" spans="1:12">
       <c r="A48" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c r="B48" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="C48" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="H48" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>169</v>
+        <v>181</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="81">
       <c r="A49" t="s">
-        <v>170</v>
+        <v>182</v>
       </c>
       <c r="B49" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="C49" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>171</v>
+        <v>183</v>
       </c>
       <c r="G49" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" t="s">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="B50" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="C50" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="D50" t="s">
-        <v>174</v>
+        <v>186</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="H50" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="J50" t="s">
-        <v>178</v>
+        <v>190</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="18" customHeight="1">
       <c r="A51" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="B51" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="C51" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="D51" t="s">
-        <v>180</v>
+        <v>192</v>
       </c>
       <c r="G51" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="18" customHeight="1">
       <c r="A52" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="B52" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="C52" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="D52" t="s">
-        <v>182</v>
+        <v>194</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="B53" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="C53" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="D53" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="H53" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="52.9">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="81">
       <c r="A54" t="s">
+        <v>199</v>
+      </c>
+      <c r="B54" t="s">
+        <v>159</v>
+      </c>
+      <c r="C54" t="s">
+        <v>160</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="G54" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B54" t="s">
-        <v>147</v>
-      </c>
-      <c r="C54" t="s">
-        <v>148</v>
-      </c>
-      <c r="D54" s="3" t="s">
+      <c r="H54" t="s">
         <v>188</v>
       </c>
-      <c r="G54" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="H54" t="s">
-        <v>176</v>
-      </c>
       <c r="I54" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="18" customHeight="1">
       <c r="A55" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="B55" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="C55" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="D55" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="G55" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="B56" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="C56" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="D56" t="s">
-        <v>192</v>
+        <v>204</v>
       </c>
       <c r="G56" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" ht="37.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="48.75">
       <c r="A57" t="s">
-        <v>193</v>
+        <v>205</v>
       </c>
       <c r="B57" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="C57" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="G57" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" ht="52.9">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="48.75">
       <c r="A58" s="2" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>197</v>
+        <v>209</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="48.75">
       <c r="A59" s="2" t="s">
-        <v>198</v>
+        <v>210</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" ht="49.35">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="48.75">
       <c r="A60" s="2" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>201</v>
+        <v>213</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="2" t="s">
-        <v>202</v>
+        <v>214</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="G61" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C61" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="G61" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10">
+    </row>
+    <row r="62" spans="1:10" ht="16.5">
       <c r="A62" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="B62" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="C62" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>208</v>
+        <v>220</v>
       </c>
       <c r="H62" t="s">
-        <v>209</v>
+        <v>221</v>
       </c>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" t="s">
-        <v>210</v>
+        <v>222</v>
       </c>
       <c r="B63" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="C63" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="D63" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>212</v>
+        <v>224</v>
       </c>
       <c r="I63" t="s">
-        <v>213</v>
+        <v>225</v>
       </c>
       <c r="J63" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="16.5" customHeight="1">
       <c r="A64" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="B64" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="C64" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>216</v>
+        <v>228</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="H64" t="s">
-        <v>218</v>
+        <v>230</v>
       </c>
     </row>
     <row r="65" spans="1:12" ht="18" customHeight="1">
       <c r="A65" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="B65" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="C65" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="H65" t="s">
-        <v>221</v>
+        <v>233</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="J65" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="K65" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="L65" s="2" t="s">
-        <v>224</v>
+        <v>236</v>
       </c>
     </row>
     <row r="66" spans="1:12" ht="18" customHeight="1">
       <c r="A66" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="B66" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="C66" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>226</v>
+        <v>238</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
     </row>
     <row r="67" spans="1:12" ht="18" customHeight="1">
       <c r="A67" t="s">
-        <v>227</v>
+        <v>239</v>
       </c>
       <c r="B67" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="C67" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>228</v>
+        <v>240</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
     </row>
     <row r="68" spans="1:12" ht="18" customHeight="1">
       <c r="A68" t="s">
-        <v>229</v>
+        <v>241</v>
       </c>
       <c r="B68" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="C68" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>230</v>
+        <v>242</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>195</v>
+        <v>207</v>
       </c>
       <c r="H68" t="s">
-        <v>231</v>
+        <v>243</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="J68" s="2" t="s">
-        <v>224</v>
+        <v>236</v>
       </c>
     </row>
     <row r="69" spans="1:12" ht="18" customHeight="1">
       <c r="A69" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="B69" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="C69" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>195</v>
+        <v>207</v>
       </c>
       <c r="H69" t="s">
-        <v>234</v>
+        <v>246</v>
       </c>
     </row>
     <row r="70" spans="1:12" ht="18" customHeight="1">
       <c r="A70" s="2" t="s">
-        <v>235</v>
+        <v>247</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>236</v>
+        <v>218</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>248</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
     </row>
     <row r="71" spans="1:12" ht="18" customHeight="1">
       <c r="A71" s="2" t="s">
-        <v>237</v>
+        <v>249</v>
       </c>
       <c r="B71" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="C71" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>238</v>
+        <v>250</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="H71" t="s">
-        <v>221</v>
+        <v>233</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="J71" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L71" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="72" spans="1:12" ht="18" customHeight="1">
       <c r="A72" s="2" t="s">
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>240</v>
+        <v>252</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="I72" s="2"/>
       <c r="K72" s="2"/>
@@ -2898,19 +2992,19 @@
     </row>
     <row r="73" spans="1:12" ht="18" customHeight="1">
       <c r="A73" s="2" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>242</v>
+        <v>254</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="H73" s="2"/>
       <c r="I73" s="2"/>
@@ -2919,333 +3013,333 @@
     </row>
     <row r="74" spans="1:12" ht="18" customHeight="1">
       <c r="A74" s="4" t="s">
-        <v>243</v>
+        <v>255</v>
       </c>
       <c r="B74" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="C74" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>246</v>
+        <v>258</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>247</v>
+        <v>259</v>
       </c>
       <c r="H74" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
     </row>
     <row r="75" spans="1:12" ht="18" customHeight="1">
       <c r="A75" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
       <c r="B75" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="C75" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>250</v>
+        <v>262</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="I75" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="J75" t="s">
-        <v>251</v>
+        <v>263</v>
       </c>
     </row>
     <row r="76" spans="1:12" ht="18" customHeight="1">
       <c r="A76" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="B76" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="C76" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>253</v>
+        <v>265</v>
       </c>
       <c r="G76" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="H76" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="I76" s="2" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="J76" s="2" t="s">
-        <v>256</v>
+        <v>268</v>
       </c>
     </row>
     <row r="77" spans="1:12" ht="15.75" customHeight="1">
       <c r="A77" t="s">
+        <v>269</v>
+      </c>
+      <c r="B77" t="s">
+        <v>256</v>
+      </c>
+      <c r="C77" t="s">
         <v>257</v>
       </c>
-      <c r="B77" t="s">
-        <v>244</v>
-      </c>
-      <c r="C77" t="s">
-        <v>245</v>
-      </c>
       <c r="D77" s="3" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="G77" t="s">
-        <v>258</v>
+        <v>270</v>
       </c>
       <c r="H77" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="I77" s="2" t="s">
-        <v>260</v>
+        <v>272</v>
       </c>
       <c r="J77" t="s">
-        <v>261</v>
+        <v>273</v>
       </c>
     </row>
     <row r="78" spans="1:12" ht="15.75" customHeight="1">
       <c r="A78" t="s">
-        <v>262</v>
+        <v>274</v>
       </c>
       <c r="B78" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="C78" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>263</v>
+        <v>275</v>
       </c>
       <c r="G78" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
       <c r="H78" s="2"/>
     </row>
     <row r="79" spans="1:12" ht="15.75" customHeight="1">
       <c r="A79" t="s">
-        <v>264</v>
+        <v>276</v>
       </c>
       <c r="B79" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="C79" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>265</v>
+        <v>277</v>
       </c>
       <c r="G79" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I79" s="2" t="s">
-        <v>266</v>
+        <v>278</v>
       </c>
       <c r="J79" t="s">
-        <v>261</v>
+        <v>273</v>
       </c>
       <c r="K79" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="L79" s="2" t="s">
-        <v>256</v>
+        <v>268</v>
       </c>
     </row>
     <row r="80" spans="1:12" ht="15.75" customHeight="1">
       <c r="A80" t="s">
-        <v>267</v>
+        <v>279</v>
       </c>
       <c r="B80" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="C80" t="s">
-        <v>268</v>
+        <v>280</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="G80" t="s">
-        <v>270</v>
+        <v>282</v>
       </c>
       <c r="I80" s="2" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="J80" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="15.75" customHeight="1">
       <c r="A81" s="2" t="s">
-        <v>273</v>
+        <v>285</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>274</v>
+        <v>286</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="15.75" customHeight="1">
       <c r="A82" s="2" t="s">
-        <v>275</v>
+        <v>287</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>277</v>
+        <v>289</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="15.75" customHeight="1">
       <c r="A83" s="2" t="s">
-        <v>278</v>
+        <v>290</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>279</v>
+        <v>291</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="H83" s="2"/>
     </row>
     <row r="84" spans="1:8" ht="15.75" customHeight="1">
       <c r="A84" t="s">
-        <v>280</v>
+        <v>292</v>
       </c>
       <c r="B84" t="s">
-        <v>280</v>
+        <v>292</v>
       </c>
       <c r="C84" t="s">
-        <v>281</v>
+        <v>293</v>
       </c>
       <c r="D84" t="s">
-        <v>282</v>
+        <v>294</v>
       </c>
       <c r="G84" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="H84" t="s">
-        <v>283</v>
+        <v>295</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="16.5" customHeight="1">
       <c r="A85" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
       <c r="B85" t="s">
-        <v>280</v>
+        <v>292</v>
       </c>
       <c r="C85" t="s">
-        <v>281</v>
+        <v>293</v>
       </c>
       <c r="D85" t="s">
-        <v>285</v>
+        <v>297</v>
       </c>
       <c r="G85" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="H85" t="s">
-        <v>283</v>
+        <v>295</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="16.5" customHeight="1">
       <c r="A86" s="2" t="s">
-        <v>286</v>
+        <v>298</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>286</v>
+        <v>298</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>287</v>
+        <v>299</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="17.25" customHeight="1">
       <c r="A87" s="2" t="s">
-        <v>289</v>
+        <v>301</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>289</v>
+        <v>301</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>290</v>
+        <v>302</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>291</v>
+        <v>303</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="17.25" customHeight="1">
       <c r="A88" s="2" t="s">
-        <v>292</v>
+        <v>304</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>292</v>
+        <v>304</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>293</v>
+        <v>305</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>294</v>
+        <v>306</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="17.25" customHeight="1">
       <c r="A89" s="2" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>296</v>
+        <v>308</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>297</v>
+        <v>309</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="15" customHeight="1">
@@ -3326,8 +3420,8 @@
   <protectedRanges>
     <protectedRange sqref="D2:D89" name="TextBox"/>
     <protectedRange sqref="G2:G89" name="Button Names"/>
-    <protectedRange sqref="I2:I89" name="Button Name 2"/>
-    <protectedRange sqref="K2:K89" name="Button Range 4"/>
+    <protectedRange sqref="K3 K7 K11 K15 K19 K23 K27 K31 K35 I2:I89" name="Button Name 2"/>
+    <protectedRange sqref="K2 K4:K6 K8:K10 K12:K14 K16:K18 K20:K22 K24:K26 K28:K30 K32:K34 K36:K89" name="Button Range 4"/>
   </protectedRanges>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Bug fixes for Cambridge
</commit_message>
<xml_diff>
--- a/cambridgeBP/dialogue/npc.xlsx
+++ b/cambridgeBP/dialogue/npc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="312">
   <si>
     <t xml:space="preserve">Scene</t>
   </si>
@@ -214,7 +214,7 @@
     <t xml:space="preserve">Deena</t>
   </si>
   <si>
-    <t xml:space="preserve">Great work you made ¾ by using ½ and ¼ , and you used the fewest rods to get here.</t>
+    <t xml:space="preserve">Great work you made 3/4 by using 1/2 and 1/4 , and you used the fewest rods to get here.</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcComplete 3</t>
@@ -661,7 +661,7 @@
     <t xml:space="preserve">scaleNpc10</t>
   </si>
   <si>
-    <t xml:space="preserve">You are true artisan, it’s time to graduate with full honours.</t>
+    <t xml:space="preserve">You are a true artisan, it’s time to graduate with full honours.</t>
   </si>
   <si>
     <t xml:space="preserve">scaleNpc11</t>
@@ -919,6 +919,9 @@
     <t xml:space="preserve">More rods</t>
   </si>
   <si>
+    <t xml:space="preserve">dialogue open @e[tag=fractionNpc] @p fractionNpc10</t>
+  </si>
+  <si>
     <t xml:space="preserve">fractionNpc6</t>
   </si>
   <si>
@@ -960,6 +963,9 @@
   </si>
   <si>
     <t xml:space="preserve">Good job! Speak to the Dean of Students to continue!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fractionNpc10</t>
   </si>
   <si>
     <t xml:space="preserve">groundskeeper</t>
@@ -1023,7 +1029,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1074,6 +1080,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1123,36 +1135,48 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1339,2099 +1363,2116 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R124"/>
+  <dimension ref="A1:R125"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D56" activeCellId="0" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="143.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="38.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="49.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="44.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="22.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="29.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="23.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="143.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="38.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="49.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="44.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="22.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="29.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="23.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="L7" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="J11" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="K11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="L11" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J15" s="3" t="s">
+      <c r="J15" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="K15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="L15" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="J17" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H18" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="I18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="J18" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="I19" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J19" s="3" t="s">
+      <c r="J19" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="K19" s="2" t="s">
+      <c r="K19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L19" s="3" t="s">
+      <c r="L19" s="4" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="I21" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="J21" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="H22" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I22" s="2" t="s">
+      <c r="I22" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J22" s="3" t="s">
+      <c r="J22" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H23" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="I23" s="2" t="s">
+      <c r="I23" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J23" s="3" t="s">
+      <c r="J23" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="K23" s="2" t="s">
+      <c r="K23" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L23" s="3" t="s">
+      <c r="L23" s="4" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G25" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I25" s="2" t="s">
+      <c r="I25" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J25" s="2" t="s">
+      <c r="J25" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="H26" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="I26" s="2" t="s">
+      <c r="I26" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J26" s="3" t="s">
+      <c r="J26" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G27" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="H27" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="I27" s="2" t="s">
+      <c r="I27" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J27" s="3" t="s">
+      <c r="J27" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K27" s="2" t="s">
+      <c r="K27" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L27" s="3" t="s">
+      <c r="L27" s="4" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G28" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G29" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G30" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H30" s="3" t="s">
+      <c r="H30" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="I30" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J30" s="3" t="s">
+      <c r="J30" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G31" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="H31" s="3" t="s">
+      <c r="H31" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="I31" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J31" s="3" t="s">
+      <c r="J31" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="K31" s="2" t="s">
+      <c r="K31" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L31" s="3" t="s">
+      <c r="L31" s="4" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="G32" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="I32" s="2" t="s">
+      <c r="I32" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J32" s="2" t="s">
+      <c r="J32" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G33" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="G34" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H34" s="3" t="s">
+      <c r="H34" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="G35" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="H35" s="3" t="s">
+      <c r="H35" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="I35" s="2" t="s">
+      <c r="I35" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J35" s="3" t="s">
+      <c r="J35" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="K35" s="2" t="s">
+      <c r="K35" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L35" s="3" t="s">
+      <c r="L35" s="4" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="G36" s="3" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="G37" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D38" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="G38" s="3" t="s">
+      <c r="G38" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="H38" s="3" t="s">
+      <c r="H38" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="I38" s="3" t="s">
+      <c r="I38" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="J38" s="3" t="s">
+      <c r="J38" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="K38" s="3" t="s">
+      <c r="K38" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="L38" s="3" t="s">
+      <c r="L38" s="4" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="G39" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="H39" s="3" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="G40" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="H40" s="3" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="G41" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="H41" s="2"/>
+      <c r="H41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="G42" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="H42" s="2"/>
+      <c r="H42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="G43" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2" t="s">
+      <c r="H43" s="3"/>
+      <c r="I43" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="J43" s="2" t="s">
+      <c r="J43" s="3" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="G44" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H44" s="2" t="s">
+      <c r="H44" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="I44" s="2" t="s">
+      <c r="I44" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="J44" s="2"/>
+      <c r="J44" s="3"/>
     </row>
     <row r="45" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B45" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="C45" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="G45" s="3" t="s">
+      <c r="G45" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H45" s="3" t="s">
+      <c r="H45" s="4" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="B46" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="C46" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D46" s="0" t="s">
+      <c r="D46" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="G46" s="0" t="s">
+      <c r="G46" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="I46" s="0" t="s">
+      <c r="I46" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="J46" s="0" t="s">
+      <c r="J46" s="1" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="B47" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C47" s="0" t="s">
+      <c r="C47" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D47" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="G47" s="3" t="s">
+      <c r="G47" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="H47" s="3" t="s">
+      <c r="H47" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="I47" s="2" t="s">
+      <c r="I47" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="J47" s="2" t="s">
+      <c r="J47" s="3" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="B48" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C48" s="0" t="s">
+      <c r="C48" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D48" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="G48" s="2" t="s">
+      <c r="G48" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H48" s="3" t="s">
+      <c r="H48" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="I48" s="2" t="s">
+      <c r="I48" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="J48" s="2" t="s">
+      <c r="J48" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="K48" s="2" t="s">
+      <c r="K48" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="L48" s="2" t="s">
+      <c r="L48" s="3" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="A49" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="B49" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C49" s="0" t="s">
+      <c r="C49" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D49" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="G49" s="3" t="s">
+      <c r="G49" s="4" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A50" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="B50" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C50" s="0" t="s">
+      <c r="C50" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D50" s="0" t="s">
+      <c r="D50" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="G50" s="2" t="s">
+      <c r="G50" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="H50" s="3" t="s">
+      <c r="H50" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="I50" s="2" t="s">
+      <c r="I50" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="J50" s="3" t="s">
+      <c r="J50" s="4" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="A51" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B51" s="0" t="s">
+      <c r="B51" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C51" s="0" t="s">
+      <c r="C51" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D51" s="0" t="s">
+      <c r="D51" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="G51" s="0" t="s">
+      <c r="G51" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="A52" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="B52" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C52" s="0" t="s">
+      <c r="C52" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D52" s="0" t="s">
+      <c r="D52" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="G52" s="2" t="s">
+      <c r="G52" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="A53" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="B53" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C53" s="0" t="s">
+      <c r="C53" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D53" s="0" t="s">
+      <c r="D53" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="G53" s="2" t="s">
+      <c r="G53" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="H53" s="3" t="s">
+      <c r="H53" s="4" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="A54" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B54" s="0" t="s">
+      <c r="B54" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C54" s="0" t="s">
+      <c r="C54" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="D54" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="G54" s="2" t="s">
+      <c r="G54" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="H54" s="3" t="s">
+      <c r="H54" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="I54" s="2" t="s">
+      <c r="I54" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J54" s="2" t="s">
+      <c r="J54" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+      <c r="A55" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B55" s="0" t="s">
+      <c r="B55" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C55" s="0" t="s">
+      <c r="C55" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D55" s="0" t="s">
+      <c r="D55" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="G55" s="0" t="s">
+      <c r="G55" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H55" s="2" t="s">
+      <c r="H55" s="3" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+      <c r="A56" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B56" s="0" t="s">
+      <c r="B56" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C56" s="0" t="s">
+      <c r="C56" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D56" s="0" t="s">
+      <c r="D56" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="G56" s="0" t="s">
+      <c r="G56" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+      <c r="A57" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B57" s="0" t="s">
+      <c r="B57" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C57" s="0" t="s">
+      <c r="C57" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D57" s="5" t="s">
+      <c r="D57" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="G57" s="3" t="s">
+      <c r="G57" s="4" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="2" t="s">
+      <c r="A58" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C58" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="D58" s="4" t="s">
+      <c r="D58" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="G58" s="2" t="s">
+      <c r="G58" s="3" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="2" t="s">
+      <c r="A59" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C59" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="D59" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="G59" s="2" t="s">
+      <c r="G59" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="H59" s="2" t="s">
+      <c r="H59" s="3" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="2" t="s">
+      <c r="A60" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="D60" s="4" t="s">
+      <c r="D60" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="G60" s="2" t="s">
+      <c r="G60" s="3" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="2" t="s">
+      <c r="A61" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B61" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C61" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="D61" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="G61" s="2" t="s">
+      <c r="G61" s="3" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+      <c r="A62" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B62" s="0" t="s">
+      <c r="B62" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C62" s="0" t="s">
+      <c r="C62" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="D62" s="4" t="s">
+      <c r="D62" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="G62" s="2" t="s">
+      <c r="G62" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="H62" s="3" t="s">
+      <c r="H62" s="4" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+      <c r="A63" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B63" s="0" t="s">
+      <c r="B63" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C63" s="0" t="s">
+      <c r="C63" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="D63" s="0" t="s">
+      <c r="D63" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="G63" s="2" t="s">
+      <c r="G63" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="I63" s="3" t="s">
+      <c r="I63" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="J63" s="3" t="s">
+      <c r="J63" s="4" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+      <c r="A64" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="B64" s="0" t="s">
+      <c r="B64" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C64" s="0" t="s">
+      <c r="C64" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="D64" s="4" t="s">
+      <c r="D64" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="G64" s="2" t="s">
+      <c r="G64" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="H64" s="3" t="s">
+      <c r="H64" s="4" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+      <c r="A65" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B65" s="0" t="s">
+      <c r="B65" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C65" s="0" t="s">
+      <c r="C65" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="D65" s="4" t="s">
+      <c r="D65" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="G65" s="2" t="s">
+      <c r="G65" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="H65" s="3" t="s">
+      <c r="H65" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="I65" s="2" t="s">
+      <c r="I65" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="J65" s="3" t="s">
+      <c r="J65" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="K65" s="3" t="s">
+      <c r="K65" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="L65" s="2" t="s">
+      <c r="L65" s="3" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+      <c r="A66" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B66" s="0" t="s">
+      <c r="B66" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C66" s="0" t="s">
+      <c r="C66" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="D66" s="4" t="s">
+      <c r="D66" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="G66" s="2" t="s">
+      <c r="G66" s="3" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+      <c r="A67" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="B67" s="0" t="s">
+      <c r="B67" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C67" s="0" t="s">
+      <c r="C67" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="D67" s="4" t="s">
+      <c r="D67" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="G67" s="2" t="s">
+      <c r="G67" s="3" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
+      <c r="A68" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="B68" s="0" t="s">
+      <c r="B68" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C68" s="0" t="s">
+      <c r="C68" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="D68" s="4" t="s">
+      <c r="D68" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="G68" s="2" t="s">
+      <c r="G68" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="H68" s="3" t="s">
+      <c r="H68" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="I68" s="2" t="s">
+      <c r="I68" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="J68" s="2" t="s">
+      <c r="J68" s="3" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+      <c r="A69" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B69" s="0" t="s">
+      <c r="B69" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C69" s="0" t="s">
+      <c r="C69" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="D69" s="4" t="s">
+      <c r="D69" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="G69" s="2" t="s">
+      <c r="G69" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="H69" s="3" t="s">
+      <c r="H69" s="4" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="2" t="s">
+      <c r="A70" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B70" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C70" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="D70" s="5" t="s">
+      <c r="D70" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="G70" s="2" t="s">
+      <c r="G70" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="H70" s="2" t="s">
+      <c r="H70" s="3" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="2" t="s">
+      <c r="A71" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B71" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="C71" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="D71" s="4" t="s">
+      <c r="D71" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="G71" s="2" t="s">
+      <c r="G71" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="H71" s="3" t="s">
+      <c r="H71" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="I71" s="2" t="s">
+      <c r="I71" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="J71" s="3" t="s">
+      <c r="J71" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="K71" s="2" t="s">
+      <c r="K71" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="L71" s="2" t="s">
+      <c r="L71" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="2" t="s">
+      <c r="A72" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B72" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C72" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="D72" s="4" t="s">
+      <c r="D72" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="G72" s="2" t="s">
+      <c r="G72" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="H72" s="2" t="s">
+      <c r="H72" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="I72" s="2"/>
-      <c r="K72" s="2"/>
-      <c r="L72" s="2"/>
+      <c r="I72" s="3"/>
+      <c r="K72" s="3"/>
+      <c r="L72" s="3"/>
     </row>
     <row r="73" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="2" t="s">
+      <c r="A73" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B73" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C73" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="D73" s="4" t="s">
+      <c r="D73" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="G73" s="2" t="s">
+      <c r="G73" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="H73" s="2"/>
-      <c r="I73" s="2"/>
-      <c r="K73" s="2"/>
-      <c r="L73" s="2"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
+      <c r="K73" s="3"/>
+      <c r="L73" s="3"/>
     </row>
     <row r="74" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="5" t="s">
+      <c r="A74" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B74" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="C74" s="3" t="s">
+      <c r="C74" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="D74" s="4" t="s">
+      <c r="D74" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="G74" s="2" t="s">
+      <c r="G74" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="H74" s="3" t="s">
+      <c r="H74" s="4" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
+      <c r="A75" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="B75" s="0" t="s">
+      <c r="B75" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="C75" s="0" t="s">
+      <c r="C75" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="D75" s="5" t="s">
+      <c r="D75" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="G75" s="2" t="s">
+      <c r="G75" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="I75" s="3" t="s">
+      <c r="I75" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="J75" s="3" t="s">
+      <c r="J75" s="4" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
+      <c r="A76" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="B76" s="0" t="s">
+      <c r="B76" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="C76" s="0" t="s">
+      <c r="C76" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="D76" s="4" t="s">
+      <c r="D76" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="G76" s="3" t="s">
+      <c r="G76" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="H76" s="3" t="s">
+      <c r="H76" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="I76" s="2" t="s">
+      <c r="I76" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="J76" s="2" t="s">
+      <c r="J76" s="3" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
+      <c r="A77" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="B77" s="0" t="s">
+      <c r="B77" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="C77" s="0" t="s">
+      <c r="C77" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="D77" s="4" t="s">
+      <c r="D77" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="G77" s="3" t="s">
+      <c r="G77" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="H77" s="3" t="s">
+      <c r="H77" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="I77" s="2" t="s">
+      <c r="I77" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="J77" s="3" t="s">
+      <c r="J77" s="4" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
+      <c r="A78" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="B78" s="0" t="s">
+      <c r="B78" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="C78" s="0" t="s">
+      <c r="C78" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="D78" s="4" t="s">
+      <c r="D78" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="G78" s="3" t="s">
+      <c r="G78" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="H78" s="2"/>
+      <c r="H78" s="3"/>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
+      <c r="A79" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="B79" s="0" t="s">
+      <c r="B79" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="C79" s="0" t="s">
+      <c r="C79" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="D79" s="4" t="s">
+      <c r="D79" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="G79" s="3" t="s">
+      <c r="G79" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I79" s="2" t="s">
+      <c r="I79" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="J79" s="3" t="s">
+      <c r="J79" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="K79" s="3" t="s">
+      <c r="K79" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="L79" s="2" t="s">
-        <v>268</v>
+      <c r="L79" s="3" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
-        <v>279</v>
-      </c>
-      <c r="B80" s="0" t="s">
+      <c r="A80" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="C80" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="D80" s="4" t="s">
+      <c r="C80" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="G80" s="3" t="s">
+      <c r="D80" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="I80" s="2" t="s">
+      <c r="G80" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="J80" s="3" t="s">
+      <c r="I80" s="3" t="s">
         <v>284</v>
       </c>
+      <c r="J80" s="4" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="2" t="s">
+      <c r="A81" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H81" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="B81" s="2" t="s">
+    </row>
+    <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A82" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="B82" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C82" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="D81" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="G81" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H81" s="2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="B82" s="2" t="s">
+      <c r="D82" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H82" s="3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A83" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B83" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="C83" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="D82" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="G82" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H82" s="2" t="s">
+      <c r="D83" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="H83" s="3"/>
+    </row>
+    <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A84" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="C84" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D84" s="10" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="D83" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="G83" s="2" t="s">
+      <c r="G84" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="H83" s="2"/>
-    </row>
-    <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
-        <v>292</v>
-      </c>
-      <c r="B84" s="0" t="s">
-        <v>292</v>
-      </c>
-      <c r="C84" s="0" t="s">
-        <v>293</v>
-      </c>
-      <c r="D84" s="0" t="s">
+      <c r="H84" s="3"/>
+    </row>
+    <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="G84" s="0" t="s">
+      <c r="B85" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="G85" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="H84" s="0" t="s">
+      <c r="H85" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C86" s="1" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="85" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
-        <v>296</v>
-      </c>
-      <c r="B85" s="0" t="s">
-        <v>292</v>
-      </c>
-      <c r="C85" s="0" t="s">
-        <v>293</v>
-      </c>
-      <c r="D85" s="0" t="s">
+      <c r="D86" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H86" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="G85" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="H85" s="0" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="D86" s="4" t="s">
+    </row>
+    <row r="87" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A87" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="G86" s="2" t="s">
+      <c r="B87" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="G87" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="D87" s="4" t="s">
+    <row r="88" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A88" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="G87" s="2" t="s">
+      <c r="B88" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="G88" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="D88" s="4" t="s">
+    <row r="89" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A89" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="G88" s="2" t="s">
+      <c r="B89" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="G89" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A89" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="D89" s="4" t="s">
+    <row r="90" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A90" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="G89" s="2" t="s">
+      <c r="B90" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="G90" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D90" s="5"/>
-    </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D91" s="5"/>
-    </row>
-    <row r="92" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D92" s="5"/>
+      <c r="D91" s="6"/>
+    </row>
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D92" s="6"/>
     </row>
     <row r="93" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D93" s="5"/>
-    </row>
-    <row r="94" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D94" s="5"/>
+      <c r="D93" s="6"/>
+    </row>
+    <row r="94" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D94" s="6"/>
     </row>
     <row r="95" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D95" s="5"/>
-    </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D96" s="5"/>
-    </row>
-    <row r="97" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D97" s="5"/>
+      <c r="D95" s="6"/>
+    </row>
+    <row r="96" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D96" s="6"/>
+    </row>
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D97" s="6"/>
     </row>
     <row r="98" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D98" s="5"/>
+      <c r="D98" s="6"/>
     </row>
     <row r="99" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D99" s="5"/>
+      <c r="D99" s="6"/>
     </row>
     <row r="100" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D100" s="5"/>
-    </row>
-    <row r="101" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D101" s="5"/>
-    </row>
-    <row r="102" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D102" s="5"/>
-    </row>
-    <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D103" s="5"/>
-    </row>
-    <row r="104" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D104" s="5"/>
-    </row>
-    <row r="105" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D105" s="5"/>
-    </row>
-    <row r="106" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D106" s="5"/>
-    </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D107" s="5"/>
-    </row>
-    <row r="108" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="D100" s="6"/>
+    </row>
+    <row r="101" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D101" s="6"/>
+    </row>
+    <row r="102" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D102" s="6"/>
+    </row>
+    <row r="103" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D103" s="6"/>
+    </row>
+    <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D104" s="6"/>
+    </row>
+    <row r="105" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D105" s="6"/>
+    </row>
+    <row r="106" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D106" s="6"/>
+    </row>
+    <row r="107" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D107" s="6"/>
+    </row>
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D108" s="6"/>
+    </row>
     <row r="109" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="110" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D110" s="5"/>
-    </row>
-    <row r="111" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="110" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="111" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D111" s="6"/>
+    </row>
     <row r="112" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="113" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="114" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3445,14 +3486,8 @@
     <row r="122" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="123" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="124" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="125" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <sheetProtection sheet="true" objects="true" scenarios="true"/>
-  <protectedRanges>
-    <protectedRange name="TextBox" sqref="D2:D89"/>
-    <protectedRange name="Button Names" sqref="G2:G89"/>
-    <protectedRange name="Button Name 2" sqref="K3 K7 K11 K15 K19 K23 K27 K31 K35 I2:I89"/>
-    <protectedRange name="Button Range 4" sqref="K2 K4:K6 K8:K10 K12:K14 K16:K18 K20:K22 K24:K26 K28:K30 K32:K34 K36:K89"/>
-  </protectedRanges>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>